<commit_message>
void till int, result till score
</commit_message>
<xml_diff>
--- a/Resultat/Decathlon.excel.xlsx
+++ b/Resultat/Decathlon.excel.xlsx
@@ -12,15 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>NAME</t>
   </si>
   <si>
     <t>Anton</t>
-  </si>
-  <si>
-    <t>Martin</t>
   </si>
 </sst>
 </file>
@@ -65,13 +62,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="25.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -84,11 +81,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Score läggs till i Excel-filen
</commit_message>
<xml_diff>
--- a/Resultat/Decathlon.excel.xlsx
+++ b/Resultat/Decathlon.excel.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>NAME</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
   <si>
     <t>Anton</t>
@@ -62,23 +65,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.0"/>
+    <col min="1" max="1" width="20.859375" customWidth="true"/>
+    <col min="2" max="2" width="9.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1100.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Discipline läggs till i Excel-filen
</commit_message>
<xml_diff>
--- a/Resultat/Decathlon.excel.xlsx
+++ b/Resultat/Decathlon.excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -20,7 +20,13 @@
     <t>Score</t>
   </si>
   <si>
+    <t>Discipline</t>
+  </si>
+  <si>
     <t>Anton</t>
+  </si>
+  <si>
+    <t>Heptathlon 100 meters hurdles</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -73,6 +79,7 @@
   <cols>
     <col min="1" max="1" width="20.859375" customWidth="true"/>
     <col min="2" max="2" width="9.140625" customWidth="true"/>
+    <col min="3" max="3" width="32.578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -82,13 +89,19 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>1100.0</v>
+        <v>1617.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nu får man välja mellan decathlon och heptathlon i början. //Joel
</commit_message>
<xml_diff>
--- a/Resultat/Decathlon.excel.xlsx
+++ b/Resultat/Decathlon.excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -23,10 +23,25 @@
     <t>Discipline</t>
   </si>
   <si>
-    <t>Anton</t>
+    <t>joel</t>
   </si>
   <si>
-    <t>Heptathlon 100 meters hurdles</t>
+    <t>Decathlon 110 meters hurdles</t>
+  </si>
+  <si>
+    <t>Heptathlon Shot Put</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Decathlon Long Jump</t>
+  </si>
+  <si>
+    <t>hugo</t>
+  </si>
+  <si>
+    <t>Heptathlon High Jump</t>
   </si>
 </sst>
 </file>
@@ -71,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -98,10 +113,43 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>1617.0</v>
+        <v>349.0</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6941.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1606.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1237.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Böt plats på Discipline och Score i excel
</commit_message>
<xml_diff>
--- a/Resultat/Decathlon.excel.xlsx
+++ b/Resultat/Decathlon.excel.xlsx
@@ -12,33 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Discipline</t>
   </si>
   <si>
     <t>Score</t>
   </si>
   <si>
-    <t>Discipline</t>
-  </si>
-  <si>
-    <t>joel</t>
-  </si>
-  <si>
-    <t>Decathlon 110 meters hurdles</t>
-  </si>
-  <si>
-    <t>Heptathlon Shot Put</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Decathlon Long Jump</t>
-  </si>
-  <si>
-    <t>hugo</t>
+    <t>Anton</t>
   </si>
   <si>
     <t>Heptathlon High Jump</t>
@@ -86,15 +71,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="20.859375" customWidth="true"/>
-    <col min="2" max="2" width="9.140625" customWidth="true"/>
-    <col min="3" max="3" width="32.578125" customWidth="true"/>
+    <col min="2" max="2" width="32.578125" customWidth="true"/>
+    <col min="3" max="3" width="9.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -112,44 +97,11 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>349.0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6941.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1606.0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="C2" t="n">
         <v>1237.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>